<commit_message>
pcb: Update Alphabot ESP32 PCB
Remove the secondary ESP32 from the PCB and add a 5V voltage regulator
to the board to convert the supplied 12V to 5V. Also add the stepper
controller directly to the board.
</commit_message>
<xml_diff>
--- a/pcb/alphabot_esp32_pcb/AlphabotESP32PCB_BOM_PCBWay.xlsx
+++ b/pcb/alphabot_esp32_pcb/AlphabotESP32PCB_BOM_PCBWay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Android_NDK\AlphabotSZUCar\AlphabotPCB_export\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Android_NDK\AlphabotSZUCar\AlphabotSZUCar\pcb\alphabot_esp32_pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6692C7E9-FB9E-4B1A-9B01-4D1E7BA80B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D22E49-B960-4B95-B29D-68DD0AC78CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="2220" windowWidth="18585" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,30 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>Item #</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ref Des</t>
-    </r>
   </si>
   <si>
     <r>
@@ -96,6 +75,177 @@
     <t>Description / Value</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Your Instructions / Notes</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Vishay / Dale</t>
+  </si>
+  <si>
+    <t>CRCW06031K00FKEA</t>
+  </si>
+  <si>
+    <t>RES 1.0K OHM 1/10W 1%</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>CRCW060310K0FKEA</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1/10W 1%</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1uF ±10% 25V X7R</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>ICMU1</t>
+  </si>
+  <si>
+    <t>ICM-20948</t>
+  </si>
+  <si>
+    <t>TDK InvenSense</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>ICMC1</t>
+  </si>
+  <si>
+    <t>Q1,Q3,Q4</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>R5,R6,R7,R11</t>
+  </si>
+  <si>
+    <t>R9,R10</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>BSS138</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>C0603C104K3RAC7013</t>
+  </si>
+  <si>
+    <t>C0603C106M8PAC7411</t>
+  </si>
+  <si>
+    <t>CAP CER 10uF ±20% 10V X5R</t>
+  </si>
+  <si>
+    <t>C0805C104K5RAC7411</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1uF ±10% 50V X7R</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>CRCW06032K20FKEA</t>
+  </si>
+  <si>
+    <t>RES 2.2K OHM 1/10W 1%</t>
+  </si>
+  <si>
+    <t>CRCW06034K70FKEA</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 1/10W 1%</t>
+  </si>
+  <si>
+    <t>MIC5225-1.8YM5-TR</t>
+  </si>
+  <si>
+    <t>Microchip Technology / Micrel</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>IMU ACCEL/GYRO/COMPI2C/SPI 24QFN</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 50V 220MA SOT23-3</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 1.8V 150MA SOT-23-5</t>
+  </si>
+  <si>
+    <t>24QFN</t>
+  </si>
+  <si>
+    <t>18-SOP</t>
+  </si>
+  <si>
+    <t>SOP-18 DARLINGTON TRANSISTOR ARR</t>
+  </si>
+  <si>
+    <t>ULN2803A</t>
+  </si>
+  <si>
+    <t>UTD Semiconductor</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>D2PAK</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 5V 1.5A D2PAK</t>
+  </si>
+  <si>
+    <t>L7805ACD2T-TR</t>
+  </si>
+  <si>
+    <t>CAP CER 330PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>C0603C331K5RAC7867</t>
+  </si>
+  <si>
+    <t>C1,C4</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -113,147 +263,39 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Package</t>
+      <t>Designator</t>
     </r>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Your Instructions / Notes</t>
-  </si>
-  <si>
-    <t>SMD</t>
-  </si>
-  <si>
-    <t>0603</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>Vishay / Dale</t>
-  </si>
-  <si>
-    <t>CRCW06031K00FKEA</t>
-  </si>
-  <si>
-    <t>RES 1.0K OHM 1/10W 1%</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>CRCW060310K0FKEA</t>
-  </si>
-  <si>
-    <t>RES 10K OHM 1/10W 1%</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1uF ±10% 25V X7R</t>
-  </si>
-  <si>
-    <t>BOM</t>
-  </si>
-  <si>
-    <t>ICMU1</t>
-  </si>
-  <si>
-    <t>ICM-20948</t>
-  </si>
-  <si>
-    <t>TDK InvenSense</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>ICMC1</t>
-  </si>
-  <si>
-    <t>Q1,Q3,Q4</t>
-  </si>
-  <si>
-    <t>ON Semiconductor</t>
-  </si>
-  <si>
-    <t>R5,R6,R7,R11</t>
-  </si>
-  <si>
-    <t>R9,R10</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>BSS138</t>
-  </si>
-  <si>
-    <t>KEMET</t>
-  </si>
-  <si>
-    <t>C0603C104K3RAC7013</t>
-  </si>
-  <si>
-    <t>C0603C106M8PAC7411</t>
-  </si>
-  <si>
-    <t>CAP CER 10uF ±20% 10V X5R</t>
-  </si>
-  <si>
-    <t>C0805C104K5RAC7411</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1uF ±10% 50V X7R</t>
-  </si>
-  <si>
-    <t>0805</t>
-  </si>
-  <si>
-    <t>CRCW06032K20FKEA</t>
-  </si>
-  <si>
-    <t>RES 2.2K OHM 1/10W 1%</t>
-  </si>
-  <si>
-    <t>CRCW06034K70FKEA</t>
-  </si>
-  <si>
-    <t>RES 4.7K OHM 1/10W 1%</t>
-  </si>
-  <si>
-    <t>MIC5225-1.8YM5-TR</t>
-  </si>
-  <si>
-    <t>Microchip Technology / Micrel</t>
-  </si>
-  <si>
-    <t>SOT-23-5</t>
-  </si>
-  <si>
-    <t>SOT-23-3</t>
-  </si>
-  <si>
-    <t>IMU ACCEL/GYRO/COMPI2C/SPI 24QFN</t>
-  </si>
-  <si>
-    <t>MOSFET N-CH 50V 220MA SOT23-3</t>
-  </si>
-  <si>
-    <t>IC REG LINEAR 1.8V 150MA SOT-23-5</t>
-  </si>
-  <si>
-    <t>24QFN</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Package/Footprint</t>
+    </r>
+  </si>
+  <si>
+    <t>Pin 1 is on the left side. It is intentional that there is no pad on the PCB for the exposed die pad on the center of the chip.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,13 +328,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
@@ -307,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +352,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,16 +386,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -377,9 +414,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -389,9 +423,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -741,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I17"/>
+  <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -755,60 +794,60 @@
     <col min="4" max="4" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="35.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="103.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="D2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="D2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -816,52 +855,54 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3">
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I8" s="6"/>
     </row>
@@ -870,25 +911,25 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="G9" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I9" s="6"/>
     </row>
@@ -897,25 +938,25 @@
         <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I10" s="6"/>
     </row>
@@ -924,25 +965,25 @@
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3">
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I11" s="6"/>
     </row>
@@ -951,25 +992,25 @@
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="G12" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I12" s="6"/>
     </row>
@@ -978,25 +1019,25 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I13" s="6"/>
     </row>
@@ -1005,25 +1046,25 @@
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3">
         <v>4</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I14" s="6"/>
     </row>
@@ -1032,25 +1073,25 @@
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3">
         <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I15" s="6"/>
     </row>
@@ -1059,48 +1100,121 @@
         <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="3">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
+      <c r="G17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="3">
+        <v>12</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="3">
+        <v>13</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D18" r:id="rId1" display="https://www.mouser.at/manufacturer/stmicroelectronics/" xr:uid="{5667F418-C212-4609-B90D-1DEC36C0E137}"/>
+  </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1112,7 +1226,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
 </worksheet>
@@ -1126,7 +1240,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
pcb: Update Alphabot ESP32 PCB (#116)
Remove the secondary ESP32 from the PCB and add a 5V voltage regulator
to the board to convert the supplied 12V to 5V. Also add the stepper
controller directly to the board.
</commit_message>
<xml_diff>
--- a/pcb/alphabot_esp32_pcb/AlphabotESP32PCB_BOM_PCBWay.xlsx
+++ b/pcb/alphabot_esp32_pcb/AlphabotESP32PCB_BOM_PCBWay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Android_NDK\AlphabotSZUCar\AlphabotPCB_export\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Android_NDK\AlphabotSZUCar\AlphabotSZUCar\pcb\alphabot_esp32_pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6692C7E9-FB9E-4B1A-9B01-4D1E7BA80B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D22E49-B960-4B95-B29D-68DD0AC78CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="2220" windowWidth="18585" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,30 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>Item #</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ref Des</t>
-    </r>
   </si>
   <si>
     <r>
@@ -96,6 +75,177 @@
     <t>Description / Value</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Your Instructions / Notes</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Vishay / Dale</t>
+  </si>
+  <si>
+    <t>CRCW06031K00FKEA</t>
+  </si>
+  <si>
+    <t>RES 1.0K OHM 1/10W 1%</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>CRCW060310K0FKEA</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1/10W 1%</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1uF ±10% 25V X7R</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>ICMU1</t>
+  </si>
+  <si>
+    <t>ICM-20948</t>
+  </si>
+  <si>
+    <t>TDK InvenSense</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>ICMC1</t>
+  </si>
+  <si>
+    <t>Q1,Q3,Q4</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>R5,R6,R7,R11</t>
+  </si>
+  <si>
+    <t>R9,R10</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>BSS138</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>C0603C104K3RAC7013</t>
+  </si>
+  <si>
+    <t>C0603C106M8PAC7411</t>
+  </si>
+  <si>
+    <t>CAP CER 10uF ±20% 10V X5R</t>
+  </si>
+  <si>
+    <t>C0805C104K5RAC7411</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1uF ±10% 50V X7R</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>CRCW06032K20FKEA</t>
+  </si>
+  <si>
+    <t>RES 2.2K OHM 1/10W 1%</t>
+  </si>
+  <si>
+    <t>CRCW06034K70FKEA</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 1/10W 1%</t>
+  </si>
+  <si>
+    <t>MIC5225-1.8YM5-TR</t>
+  </si>
+  <si>
+    <t>Microchip Technology / Micrel</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>IMU ACCEL/GYRO/COMPI2C/SPI 24QFN</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 50V 220MA SOT23-3</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 1.8V 150MA SOT-23-5</t>
+  </si>
+  <si>
+    <t>24QFN</t>
+  </si>
+  <si>
+    <t>18-SOP</t>
+  </si>
+  <si>
+    <t>SOP-18 DARLINGTON TRANSISTOR ARR</t>
+  </si>
+  <si>
+    <t>ULN2803A</t>
+  </si>
+  <si>
+    <t>UTD Semiconductor</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>D2PAK</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 5V 1.5A D2PAK</t>
+  </si>
+  <si>
+    <t>L7805ACD2T-TR</t>
+  </si>
+  <si>
+    <t>CAP CER 330PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>C0603C331K5RAC7867</t>
+  </si>
+  <si>
+    <t>C1,C4</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -113,147 +263,39 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Package</t>
+      <t>Designator</t>
     </r>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Your Instructions / Notes</t>
-  </si>
-  <si>
-    <t>SMD</t>
-  </si>
-  <si>
-    <t>0603</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>Vishay / Dale</t>
-  </si>
-  <si>
-    <t>CRCW06031K00FKEA</t>
-  </si>
-  <si>
-    <t>RES 1.0K OHM 1/10W 1%</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>CRCW060310K0FKEA</t>
-  </si>
-  <si>
-    <t>RES 10K OHM 1/10W 1%</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1uF ±10% 25V X7R</t>
-  </si>
-  <si>
-    <t>BOM</t>
-  </si>
-  <si>
-    <t>ICMU1</t>
-  </si>
-  <si>
-    <t>ICM-20948</t>
-  </si>
-  <si>
-    <t>TDK InvenSense</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>ICMC1</t>
-  </si>
-  <si>
-    <t>Q1,Q3,Q4</t>
-  </si>
-  <si>
-    <t>ON Semiconductor</t>
-  </si>
-  <si>
-    <t>R5,R6,R7,R11</t>
-  </si>
-  <si>
-    <t>R9,R10</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>BSS138</t>
-  </si>
-  <si>
-    <t>KEMET</t>
-  </si>
-  <si>
-    <t>C0603C104K3RAC7013</t>
-  </si>
-  <si>
-    <t>C0603C106M8PAC7411</t>
-  </si>
-  <si>
-    <t>CAP CER 10uF ±20% 10V X5R</t>
-  </si>
-  <si>
-    <t>C0805C104K5RAC7411</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1uF ±10% 50V X7R</t>
-  </si>
-  <si>
-    <t>0805</t>
-  </si>
-  <si>
-    <t>CRCW06032K20FKEA</t>
-  </si>
-  <si>
-    <t>RES 2.2K OHM 1/10W 1%</t>
-  </si>
-  <si>
-    <t>CRCW06034K70FKEA</t>
-  </si>
-  <si>
-    <t>RES 4.7K OHM 1/10W 1%</t>
-  </si>
-  <si>
-    <t>MIC5225-1.8YM5-TR</t>
-  </si>
-  <si>
-    <t>Microchip Technology / Micrel</t>
-  </si>
-  <si>
-    <t>SOT-23-5</t>
-  </si>
-  <si>
-    <t>SOT-23-3</t>
-  </si>
-  <si>
-    <t>IMU ACCEL/GYRO/COMPI2C/SPI 24QFN</t>
-  </si>
-  <si>
-    <t>MOSFET N-CH 50V 220MA SOT23-3</t>
-  </si>
-  <si>
-    <t>IC REG LINEAR 1.8V 150MA SOT-23-5</t>
-  </si>
-  <si>
-    <t>24QFN</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Package/Footprint</t>
+    </r>
+  </si>
+  <si>
+    <t>Pin 1 is on the left side. It is intentional that there is no pad on the PCB for the exposed die pad on the center of the chip.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,13 +328,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
@@ -307,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +352,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,16 +386,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -377,9 +414,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -389,9 +423,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -741,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I17"/>
+  <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -755,60 +794,60 @@
     <col min="4" max="4" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="35.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="103.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="D2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="D2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -816,52 +855,54 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3">
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I8" s="6"/>
     </row>
@@ -870,25 +911,25 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="G9" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I9" s="6"/>
     </row>
@@ -897,25 +938,25 @@
         <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I10" s="6"/>
     </row>
@@ -924,25 +965,25 @@
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3">
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I11" s="6"/>
     </row>
@@ -951,25 +992,25 @@
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="G12" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I12" s="6"/>
     </row>
@@ -978,25 +1019,25 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I13" s="6"/>
     </row>
@@ -1005,25 +1046,25 @@
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3">
         <v>4</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I14" s="6"/>
     </row>
@@ -1032,25 +1073,25 @@
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3">
         <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I15" s="6"/>
     </row>
@@ -1059,48 +1100,121 @@
         <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="3">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
+      <c r="G17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="3">
+        <v>12</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="3">
+        <v>13</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D18" r:id="rId1" display="https://www.mouser.at/manufacturer/stmicroelectronics/" xr:uid="{5667F418-C212-4609-B90D-1DEC36C0E137}"/>
+  </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1112,7 +1226,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
 </worksheet>
@@ -1126,7 +1240,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
 </worksheet>

</xml_diff>